<commit_message>
add more query detail and capability statement
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.BlueBundle.xlsx
+++ b/docs/StructureDefinition-VA.MHV.BlueBundle.xlsx
@@ -87,14 +87,14 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">A profile on the Bundle that declares how MHV will Create/Update in PGHD for BlueButton report.
+    <t>A profile on the Bundle that declares how MHV will Create/Update in PGHD for BlueButton report.
 **This is a work in progress. It is not agreed to, and it is not ready for review.**
 * must be a document type Bundle
 * must have a timestamp of when this was created
 * must have a MHV Bluebutton type of a Composition 
 * must include Patient Resource
 * must include all Resources referenced by Composition 
-* DSTU2 use comment rather than note </t>
+* DSTU2 use comment rather than note</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>